<commit_message>
12th May 2023 Backend
</commit_message>
<xml_diff>
--- a/app/ReportGeneration/EnergyData.xlsx
+++ b/app/ReportGeneration/EnergyData.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="reactiveHigh" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="activeHigh" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,500 +450,269 @@
           <t>FK-02</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>FK-03</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>43831</v>
+        <v>43101</v>
       </c>
       <c r="B2" t="n">
-        <v>-445.4</v>
+        <v>11384.1816</v>
       </c>
       <c r="C2" t="n">
-        <v>-954.7</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
+        <v>-11146.3635</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>43832</v>
+        <v>43102</v>
       </c>
       <c r="B3" t="n">
-        <v>-466.7</v>
+        <v>10363.6362</v>
       </c>
       <c r="C3" t="n">
-        <v>-773.4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
+        <v>-11090.1816</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>43833</v>
+        <v>43103</v>
       </c>
       <c r="B4" t="n">
-        <v>-510.9</v>
+        <v>11646.5451</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
+        <v>-11687.9997</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>43834</v>
+        <v>43104</v>
       </c>
       <c r="B5" t="n">
-        <v>-490.5</v>
+        <v>11983.6362</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
+        <v>-11803.0905</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>43835</v>
+        <v>43105</v>
       </c>
       <c r="B6" t="n">
-        <v>-495.2</v>
+        <v>12686.727</v>
       </c>
       <c r="C6" t="n">
-        <v>-729.8</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
+        <v>-12612.5451</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>43836</v>
+        <v>43106</v>
       </c>
       <c r="B7" t="n">
-        <v>-483</v>
+        <v>11549.4543</v>
       </c>
       <c r="C7" t="n">
-        <v>-619.8</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
+        <v>-12188.727</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>43837</v>
+        <v>43107</v>
       </c>
       <c r="B8" t="n">
-        <v>-392.7</v>
+        <v>10735.6362</v>
       </c>
       <c r="C8" t="n">
-        <v>235.6</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
+        <v>-11866.9089</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>43838</v>
+        <v>43108</v>
       </c>
       <c r="B9" t="n">
-        <v>-449.2</v>
+        <v>10728.5451</v>
       </c>
       <c r="C9" t="n">
-        <v>66.5</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
+        <v>-11495.9997</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>43839</v>
+        <v>43109</v>
       </c>
       <c r="B10" t="n">
-        <v>-466.7</v>
+        <v>10675.6362</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.3</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
+        <v>-11453.9997</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>43840</v>
+        <v>43110</v>
       </c>
       <c r="B11" t="n">
-        <v>-464.9</v>
+        <v>11777.9997</v>
       </c>
       <c r="C11" t="n">
-        <v>21.8</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
+        <v>-11576.727</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>43841</v>
+        <v>43111</v>
       </c>
       <c r="B12" t="n">
-        <v>-464.5</v>
+        <v>12622.9089</v>
       </c>
       <c r="C12" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
+        <v>-8600.727000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>43842</v>
+        <v>43112</v>
       </c>
       <c r="B13" t="n">
-        <v>-474.7</v>
+        <v>12234.5451</v>
       </c>
       <c r="C13" t="n">
-        <v>-22.5</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
+        <v>-12476.1816</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>43843</v>
+        <v>43113</v>
       </c>
       <c r="B14" t="n">
-        <v>-386.3</v>
+        <v>12176.727</v>
       </c>
       <c r="C14" t="n">
-        <v>78.7</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
+        <v>-12475.6362</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>43844</v>
+        <v>43114</v>
       </c>
       <c r="B15" t="n">
-        <v>-475.4</v>
+        <v>12407.4543</v>
       </c>
       <c r="C15" t="n">
-        <v>-21.4</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
+        <v>-12771.8178</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>43845</v>
+        <v>43115</v>
       </c>
       <c r="B16" t="n">
-        <v>-440.5</v>
+        <v>11701.6362</v>
       </c>
       <c r="C16" t="n">
-        <v>10.3</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
+        <v>-12089.4543</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>43846</v>
+        <v>43116</v>
       </c>
       <c r="B17" t="n">
-        <v>-497</v>
+        <v>11402.1816</v>
       </c>
       <c r="C17" t="n">
-        <v>-79</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
+        <v>-11735.4543</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>43847</v>
+        <v>43117</v>
       </c>
       <c r="B18" t="n">
-        <v>-343.8</v>
+        <v>11638.9089</v>
       </c>
       <c r="C18" t="n">
-        <v>-142.7</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
+        <v>-11824.3635</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>43848</v>
+        <v>43118</v>
       </c>
       <c r="B19" t="n">
-        <v>-227.8</v>
+        <v>11607.8178</v>
       </c>
       <c r="C19" t="n">
-        <v>-125.9</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
+        <v>-11828.1816</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>43849</v>
+        <v>43119</v>
       </c>
       <c r="B20" t="n">
-        <v>-257.6</v>
+        <v>11382.5451</v>
       </c>
       <c r="C20" t="n">
-        <v>-316.1</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
+        <v>-11829.2724</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>43850</v>
+        <v>43120</v>
       </c>
       <c r="B21" t="n">
-        <v>-208.3</v>
+        <v>11392.9089</v>
       </c>
       <c r="C21" t="n">
-        <v>-287.9</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
+        <v>-11533.0905</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>43851</v>
+        <v>43121</v>
       </c>
       <c r="B22" t="n">
-        <v>-197.9</v>
+        <v>10279.0908</v>
       </c>
       <c r="C22" t="n">
-        <v>-515.2</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
+        <v>-10279.0908</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>43852</v>
+        <v>43122</v>
       </c>
       <c r="B23" t="n">
-        <v>-182.9</v>
+        <v>10979.9997</v>
       </c>
       <c r="C23" t="n">
-        <v>-399.4</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
+        <v>-11042.1816</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>43853</v>
+        <v>43123</v>
       </c>
       <c r="B24" t="n">
-        <v>-179</v>
+        <v>8191.0908</v>
       </c>
       <c r="C24" t="n">
-        <v>-416.1</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
+        <v>-11720.1816</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>43854</v>
+        <v>43124</v>
       </c>
       <c r="B25" t="n">
-        <v>-191</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>-415</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="n">
-        <v>43855</v>
-      </c>
-      <c r="B26" t="n">
-        <v>-203.2</v>
-      </c>
-      <c r="C26" t="n">
-        <v>-401.6</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="n">
-        <v>43856</v>
-      </c>
-      <c r="B27" t="n">
-        <v>-189.2</v>
-      </c>
-      <c r="C27" t="n">
-        <v>-439</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="n">
-        <v>43857</v>
-      </c>
-      <c r="B28" t="n">
-        <v>-205.2</v>
-      </c>
-      <c r="C28" t="n">
-        <v>-427.8</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="n">
-        <v>43858</v>
-      </c>
-      <c r="B29" t="n">
-        <v>-182.3</v>
-      </c>
-      <c r="C29" t="n">
-        <v>-439.9</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="n">
-        <v>43859</v>
-      </c>
-      <c r="B30" t="n">
-        <v>-585.9</v>
-      </c>
-      <c r="C30" t="n">
-        <v>-680.5</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="n">
-        <v>43860</v>
-      </c>
-      <c r="B31" t="n">
-        <v>-652.1</v>
-      </c>
-      <c r="C31" t="n">
-        <v>-289.4</v>
-      </c>
-      <c r="D31" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="n">
-        <v>43861</v>
-      </c>
-      <c r="B32" t="n">
-        <v>-680.1</v>
-      </c>
-      <c r="C32" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="n">
-        <v>43862</v>
-      </c>
-      <c r="B33" t="n">
-        <v>-608.3</v>
-      </c>
-      <c r="C33" t="n">
-        <v>-918.9</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="n">
-        <v>43863</v>
-      </c>
-      <c r="B34" t="n">
-        <v>-660.9</v>
-      </c>
-      <c r="C34" t="n">
-        <v>-854.1</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="n">
-        <v>43864</v>
-      </c>
-      <c r="B35" t="n">
-        <v>-624.5</v>
-      </c>
-      <c r="C35" t="n">
-        <v>-846.5</v>
-      </c>
-      <c r="D35" t="n">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="n">
-        <v>43865</v>
-      </c>
-      <c r="B36" t="n">
-        <v>-691.9</v>
-      </c>
-      <c r="C36" t="n">
-        <v>-896.5</v>
-      </c>
-      <c r="D36" t="n">
-        <v>-0.7</v>
+        <v>-11287.0905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>